<commit_message>
change map format from char[][] to JSONArray(JSONArray(Char))
</commit_message>
<xml_diff>
--- a/formats.xlsx
+++ b/formats.xlsx
@@ -67,7 +67,7 @@
     <t xml:space="preserve">word</t>
   </si>
   <si>
-    <t xml:space="preserve">map (2D JsonArray?)</t>
+    <t xml:space="preserve">map (2D-JsonArray(char))</t>
   </si>
   <si>
     <t xml:space="preserve">map</t>
@@ -148,6 +148,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -207,8 +208,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -236,7 +241,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -314,7 +319,7 @@
       <c r="G7" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>16</v>
       </c>
       <c r="J7" s="0" t="s">
@@ -331,10 +336,10 @@
       <c r="E8" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J8" s="0" t="s">
@@ -345,13 +350,13 @@
       <c r="B9" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -433,7 +438,7 @@
       <c r="G18" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="1"/>
+      <c r="H18" s="2"/>
       <c r="J18" s="0" t="s">
         <v>16</v>
       </c>
@@ -448,8 +453,8 @@
       <c r="E19" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="1"/>
-      <c r="I19" s="1"/>
+      <c r="F19" s="2"/>
+      <c r="I19" s="2"/>
       <c r="J19" s="0" t="s">
         <v>19</v>
       </c>
@@ -458,8 +463,8 @@
       <c r="B20" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="H20" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">

</xml_diff>